<commit_message>
edit reviews table to reviews_update
</commit_message>
<xml_diff>
--- a/db/reviews_update_left.xlsx
+++ b/db/reviews_update_left.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15420" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>NULL</t>
   </si>
@@ -186,6 +187,53 @@
   </si>
   <si>
     <t>,1,2017-04-07 11:38:39"</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">縺ゅ≠
+</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>aaabbb</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a
+</t>
+  </si>
+  <si>
+    <t>rate</t>
   </si>
 </sst>
 </file>
@@ -511,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U110"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -771,4 +819,1077 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42832.485173611109</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42832.485173611109</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42832.489745370367</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42832.489745370367</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42832.490104166667</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42832.490104166667</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42832.49013888889</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42832.49013888889</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42832.50304398148</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42832.50304398148</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="D7" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="D9" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="D10" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42833.275671296295</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42834.250648148147</v>
+      </c>
+      <c r="D12" s="1">
+        <v>42834.250648148147</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42834.252662037034</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42834.252662037034</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42834.253113425926</v>
+      </c>
+      <c r="D14" s="1">
+        <v>42834.253113425926</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42834.253113425926</v>
+      </c>
+      <c r="D15" s="1">
+        <v>42834.253113425926</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42872.617581018516</v>
+      </c>
+      <c r="D16" s="1">
+        <v>42872.617581018516</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42872.617696759262</v>
+      </c>
+      <c r="D17" s="1">
+        <v>42872.617696759262</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42872.617777777778</v>
+      </c>
+      <c r="D18" s="1">
+        <v>42872.617777777778</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42872.619074074071</v>
+      </c>
+      <c r="D19" s="1">
+        <v>42872.619074074071</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42872.619143518517</v>
+      </c>
+      <c r="D20" s="1">
+        <v>42872.619143518517</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1">
+        <v>42872.640104166669</v>
+      </c>
+      <c r="D21" s="1">
+        <v>42872.640104166669</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42872.640162037038</v>
+      </c>
+      <c r="D22" s="1">
+        <v>42872.640162037038</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42872.640219907407</v>
+      </c>
+      <c r="D23" s="1">
+        <v>42872.640219907407</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1">
+        <v>42872.640266203707</v>
+      </c>
+      <c r="D24" s="1">
+        <v>42872.640266203707</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42872.640347222223</v>
+      </c>
+      <c r="D25" s="1">
+        <v>42872.640347222223</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
+        <v>42872.640416666669</v>
+      </c>
+      <c r="D26" s="1">
+        <v>42872.640416666669</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1">
+        <v>42872.640462962961</v>
+      </c>
+      <c r="D27" s="1">
+        <v>42872.640462962961</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42872.640648148146</v>
+      </c>
+      <c r="D28" s="1">
+        <v>42872.640648148146</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1">
+        <v>42872.640694444446</v>
+      </c>
+      <c r="D29" s="1">
+        <v>42872.640694444446</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
+        <v>42872.640740740739</v>
+      </c>
+      <c r="D30" s="1">
+        <v>42872.640740740739</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1">
+        <v>42875.218101851853</v>
+      </c>
+      <c r="D31" s="1">
+        <v>42875.218101851853</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1">
+        <v>42875.218229166669</v>
+      </c>
+      <c r="D32" s="1">
+        <v>42875.218229166669</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1">
+        <v>42875.218333333331</v>
+      </c>
+      <c r="D33" s="1">
+        <v>42875.218333333331</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1">
+        <v>42875.218425925923</v>
+      </c>
+      <c r="D34" s="1">
+        <v>42875.218425925923</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1">
+        <v>42875.218622685185</v>
+      </c>
+      <c r="D35" s="1">
+        <v>42875.218622685185</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1">
+        <v>42875.218773148146</v>
+      </c>
+      <c r="D36" s="1">
+        <v>42875.218773148146</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1">
+        <v>42875.218900462962</v>
+      </c>
+      <c r="D37" s="1">
+        <v>42875.218900462962</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1">
+        <v>42875.218993055554</v>
+      </c>
+      <c r="D38" s="1">
+        <v>42875.218993055554</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1">
+        <v>42875.219085648147</v>
+      </c>
+      <c r="D39" s="1">
+        <v>42875.219085648147</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1">
+        <v>42875.249548611115</v>
+      </c>
+      <c r="D40" s="1">
+        <v>42875.249548611115</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41">
+        <v>39</v>
+      </c>
+      <c r="C41" s="1">
+        <v>42875.249618055554</v>
+      </c>
+      <c r="D41" s="1">
+        <v>42875.249618055554</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42" s="1">
+        <v>42875.249675925923</v>
+      </c>
+      <c r="D42" s="1">
+        <v>42875.249675925923</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1">
+        <v>42875.249722222223</v>
+      </c>
+      <c r="D43" s="1">
+        <v>42875.249722222223</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1">
+        <v>42875.249768518515</v>
+      </c>
+      <c r="D44" s="1">
+        <v>42875.249768518515</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1">
+        <v>42875.249803240738</v>
+      </c>
+      <c r="D45" s="1">
+        <v>42875.249803240738</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46">
+        <v>29</v>
+      </c>
+      <c r="C46" s="1">
+        <v>42875.335902777777</v>
+      </c>
+      <c r="D46" s="1">
+        <v>42875.335902777777</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="C47" s="1">
+        <v>42875.378020833334</v>
+      </c>
+      <c r="D47" s="1">
+        <v>42875.378020833334</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="C48" s="1">
+        <v>42875.378101851849</v>
+      </c>
+      <c r="D48" s="1">
+        <v>42875.378101851849</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49">
+        <v>46</v>
+      </c>
+      <c r="C49" s="1">
+        <v>42875.378148148149</v>
+      </c>
+      <c r="D49" s="1">
+        <v>42875.378148148149</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1">
+        <v>42875.378206018519</v>
+      </c>
+      <c r="D50" s="1">
+        <v>42875.378206018519</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51">
+        <v>48</v>
+      </c>
+      <c r="C51" s="1">
+        <v>42875.378263888888</v>
+      </c>
+      <c r="D51" s="1">
+        <v>42875.378263888888</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="C52" s="1">
+        <v>42875.378321759257</v>
+      </c>
+      <c r="D52" s="1">
+        <v>42875.378321759257</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="C53" s="1">
+        <v>42875.378368055557</v>
+      </c>
+      <c r="D53" s="1">
+        <v>42875.378368055557</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>